<commit_message>
đổi điện trở WDog
</commit_message>
<xml_diff>
--- a/03_BOM/obc_ver111.xlsx
+++ b/03_BOM/obc_ver111.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Altium_Project\7_OBC_V111\NANORACK_V2_OBC_1.1.1_HW\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3568FA8-7D4C-4CE1-9F14-D5EEB4AE292B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032D030F-E2A2-4B3F-B64D-154FBBF03D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{501C5112-30DE-4070-BFC7-62D473800991}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15885" xr2:uid="{501C5112-30DE-4070-BFC7-62D473800991}"/>
   </bookViews>
   <sheets>
     <sheet name="obc_ver111" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="239">
   <si>
     <t>Name</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>J2, J5, J17</t>
-  </si>
-  <si>
     <t>JP1-D1T</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>RES</t>
   </si>
   <si>
-    <t>R1, R2, R3, R24, R25, R26, R27, R31, R44, R60, R62, R64, R65, R66, R68, R69, R82, R83, R87, R109</t>
-  </si>
-  <si>
     <t>RES_C_1608X60</t>
   </si>
   <si>
@@ -341,24 +335,12 @@
     <t>0R/1%</t>
   </si>
   <si>
-    <t>19.1k/1%</t>
-  </si>
-  <si>
-    <t>RES SMD 19.1K OHM 1% 1/10W 0603, P/N: ERJ-3EKF1912V</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
     <t>16.5k/1%</t>
   </si>
   <si>
     <t>RES SMD 16.5K OHM 1% 1/10W 0603, P/N: ERJ-3EKF1652V</t>
   </si>
   <si>
-    <t>R19</t>
-  </si>
-  <si>
     <t>4.7k/DNP</t>
   </si>
   <si>
@@ -425,9 +407,6 @@
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>LMS1587ISX-3.3/NOPB</t>
-  </si>
-  <si>
     <t>3A Low Dropout Fast Response Regulators, 3-pin TO-263, Pb-Free</t>
   </si>
   <si>
@@ -695,9 +674,6 @@
     <t>ERJ-3EKF1652V</t>
   </si>
   <si>
-    <t>ERJ-3EKF1912V</t>
-  </si>
-  <si>
     <t>ERJ-3EKF1001V</t>
   </si>
   <si>
@@ -762,6 +738,24 @@
   </si>
   <si>
     <t>1727010/DNP</t>
+  </si>
+  <si>
+    <t>LMS1585AIS-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>GRT155D70J475ME13J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đổi thành loại 5A </t>
+  </si>
+  <si>
+    <t>R19, R18</t>
+  </si>
+  <si>
+    <t>J2, J17</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R24, R25, R26, R27, R31, R44, R60, R62, R64, R65, R66, R68, R69, R82, R83, R87, R109, R55</t>
   </si>
 </sst>
 </file>
@@ -842,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -854,6 +848,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,24 +1183,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D595A2F-377A-4F1E-A2E1-7B0E47056D32}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1228,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1251,7 +1246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1297,76 +1292,76 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D7" s="1">
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -1389,7 +1384,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1412,30 +1407,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -1458,7 +1453,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -1481,30 +1476,30 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>105</v>
+        <v>236</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1527,168 +1522,168 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>102</v>
+        <v>238</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="D20" s="1">
+        <v>54</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="1">
-        <v>20</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1">
-        <v>4</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="1">
-        <v>54</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1696,13 +1691,13 @@
         <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>17</v>
@@ -1711,896 +1706,876 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D23" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>119</v>
+        <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>121</v>
+        <v>55</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>56</v>
+        <v>215</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="1">
-        <v>4</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="D28" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>184</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="F31" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="C34" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="1">
         <v>2</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="E37" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="F44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="1">
         <v>2</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="E46" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="1">
-        <v>2</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D47" s="1">
         <v>2</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D50" s="8">
         <v>2</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E50" s="8"/>
+      <c r="F50" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D51" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G51" s="8" t="s">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="H51" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D52" s="8">
-        <v>1</v>
-      </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="H52" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D55" s="1">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="1">
+        <v>3</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="1">
         <v>2</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D56" s="1">
-        <v>1</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D57" s="1">
-        <v>3</v>
-      </c>
       <c r="E57" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D58" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D59" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D61" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D62" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D63" s="1">
-        <v>4</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C64" s="7" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" s="6">
+        <v>2</v>
+      </c>
+      <c r="E63" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D64" s="6">
-        <v>2</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="G64" s="6">
+      <c r="F63" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G63" s="6">
         <v>1727010</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G50">
-    <sortCondition ref="A2:A50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G49">
+    <sortCondition ref="A2:A49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>